<commit_message>
K-Means: saidas e resultados do monkey
Co-authored-by: Bianca Gomes <bgsrd@outlook.com>
</commit_message>
<xml_diff>
--- a/k-means/resultados.xlsx
+++ b/k-means/resultados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pietrozuntini@gmail.com\Ufscar\Perfil 6\Inteligência Artificial\Trabalho IA\trabalho-ia\k-means\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pietr\Downloads\ia\k-means\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79A1757-D132-41B0-AA9E-773EE417E63C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921EC056-E296-48BE-8111-E8385FA36EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>c2ds1-2sp</t>
   </si>
@@ -65,6 +65,30 @@
   </si>
   <si>
     <t>0.2875875300901557</t>
+  </si>
+  <si>
+    <t>0.4499033097671001</t>
+  </si>
+  <si>
+    <t>0.6114212544093072</t>
+  </si>
+  <si>
+    <t>0.5717386779214773</t>
+  </si>
+  <si>
+    <t>0.7443442551221463</t>
+  </si>
+  <si>
+    <t>0.7257516640322464</t>
+  </si>
+  <si>
+    <t>0.6266431271547259</t>
+  </si>
+  <si>
+    <t>0.7019689227727416</t>
+  </si>
+  <si>
+    <t>0.578398133351854</t>
   </si>
 </sst>
 </file>
@@ -457,7 +481,7 @@
   <dimension ref="A1:AME1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -10760,7 +10784,9 @@
       <c r="A19" s="4">
         <v>5</v>
       </c>
-      <c r="B19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C19" s="2"/>
       <c r="D19" s="5"/>
       <c r="G19" s="5"/>
@@ -10769,7 +10795,9 @@
       <c r="A20" s="4">
         <v>6</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="C20" s="2"/>
       <c r="D20" s="5"/>
       <c r="G20" s="5"/>
@@ -10778,7 +10806,9 @@
       <c r="A21" s="4">
         <v>7</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="C21" s="2"/>
       <c r="D21" s="5"/>
       <c r="G21" s="5"/>
@@ -10787,7 +10817,9 @@
       <c r="A22" s="4">
         <v>8</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="C22" s="2"/>
       <c r="D22" s="5"/>
       <c r="G22" s="5"/>
@@ -10796,7 +10828,9 @@
       <c r="A23" s="4">
         <v>9</v>
       </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C23" s="2"/>
       <c r="D23" s="5"/>
       <c r="G23" s="5"/>
@@ -10805,7 +10839,9 @@
       <c r="A24" s="4">
         <v>10</v>
       </c>
-      <c r="B24" s="2"/>
+      <c r="B24" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C24" s="2"/>
       <c r="D24" s="5"/>
       <c r="G24" s="5"/>
@@ -10814,7 +10850,9 @@
       <c r="A25" s="4">
         <v>11</v>
       </c>
-      <c r="B25" s="2"/>
+      <c r="B25" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="C25" s="2"/>
       <c r="D25" s="5"/>
       <c r="G25" s="5"/>
@@ -10823,7 +10861,9 @@
       <c r="A26" s="4">
         <v>12</v>
       </c>
-      <c r="B26" s="2"/>
+      <c r="B26" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C26" s="2"/>
       <c r="D26" s="5"/>
       <c r="G26" s="5"/>

</xml_diff>